<commit_message>
various changes and supports and tests for collections
</commit_message>
<xml_diff>
--- a/tests/excel-sample/sample.xlsx
+++ b/tests/excel-sample/sample.xlsx
@@ -37,33 +37,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="3">
-    <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="20"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
+  <fonts count="1">
     <font>
       <b val="0"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
-      <sz val="15"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,15 +65,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -392,10 +368,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:SDC3"/>
+  <dimension ref="A1:SDC2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -404,30 +380,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12951">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12951">
-      <c r="A3" s="2" t="s">
+    <row r="2" spans="1:12951">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added README and support and tests for collections
</commit_message>
<xml_diff>
--- a/tests/excel-sample/sample.xlsx
+++ b/tests/excel-sample/sample.xlsx
@@ -37,33 +37,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="3">
-    <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="20"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
+  <fonts count="1">
     <font>
       <b val="0"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
-      <sz val="15"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,15 +65,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -392,10 +368,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:SDC3"/>
+  <dimension ref="A1:SDC2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -404,30 +380,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12951">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12951">
-      <c r="A3" s="2" t="s">
+    <row r="2" spans="1:12951">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bug fixes and merge fixes
</commit_message>
<xml_diff>
--- a/tests/excel-sample/sample.xlsx
+++ b/tests/excel-sample/sample.xlsx
@@ -15,21 +15,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
-  <si>
-    <t>Lorem</t>
-  </si>
-  <si>
-    <t>Ipsum</t>
-  </si>
-  <si>
-    <t>Sit</t>
-  </si>
-  <si>
-    <t>Amet</t>
-  </si>
-  <si>
-    <t>Dolore</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+  <si>
+    <t>Bill</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Stockholm</t>
+  </si>
+  <si>
+    <t>Audi</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Gothenburg</t>
+  </si>
+  <si>
+    <t>Volvo</t>
   </si>
 </sst>
 </file>
@@ -398,13 +407,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>